<commit_message>
read from/add to existing file
</commit_message>
<xml_diff>
--- a/Input/Input 3 Referred.xlsx
+++ b/Input/Input 3 Referred.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IlyaSamoylenko\Documents\UiPath Curriculum\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LevaniBukhnikashvili\Documents\UiPath\ExcellProcessor\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3AF1B843-C108-486D-AF0A-6F6C74FD7457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8ABB012-AA67-417F-837B-609086FDBE30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4A9F9BEF-0BFB-4B83-90F3-E1CA236427C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{4A9F9BEF-0BFB-4B83-90F3-E1CA236427C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>First Name</t>
   </si>
@@ -485,15 +485,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E8607A-B2C0-49E2-9004-849C5198F6B0}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +522,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -542,7 +545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -568,7 +571,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -588,6 +591,29 @@
         <v>8</v>
       </c>
       <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>